<commit_message>
hoan thanh bai tap 1
</commit_message>
<xml_diff>
--- a/src/main/java/org/people.xlsx
+++ b/src/main/java/org/people.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/working/he thong cong nghe thong tn/bai tap quan ly ngan hang/untitled/src/main/java/org/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4100AC65-BB57-C24B-8754-FE5DB38B9B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F10377-E040-824D-810A-56AE9F331F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="1640" windowWidth="38400" windowHeight="19400" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="860" windowWidth="38400" windowHeight="19400" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="people" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="nganhhoc" sheetId="7" r:id="rId4"/>
     <sheet name="KHOA" sheetId="8" r:id="rId5"/>
     <sheet name="hang xe oto " sheetId="9" r:id="rId6"/>
+    <sheet name="quanlynhanvien" sheetId="10" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'hang xe oto '!$A$1:$F$160</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9298" uniqueCount="5753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9702" uniqueCount="6140">
   <si>
     <t>Email</t>
   </si>
@@ -17301,6 +17302,1167 @@
   </si>
   <si>
     <t>MKT</t>
+  </si>
+  <si>
+    <t>madinhdanh</t>
+  </si>
+  <si>
+    <t>hoten</t>
+  </si>
+  <si>
+    <t>namsinh</t>
+  </si>
+  <si>
+    <t>he so luong</t>
+  </si>
+  <si>
+    <t>M2BHWM</t>
+  </si>
+  <si>
+    <t>Dang Khanh Duy</t>
+  </si>
+  <si>
+    <t>ZRZZLQ</t>
+  </si>
+  <si>
+    <t>Vu Phuong Lan</t>
+  </si>
+  <si>
+    <t>HZI75J</t>
+  </si>
+  <si>
+    <t>Dang Quang Khanh</t>
+  </si>
+  <si>
+    <t>OZVMLV</t>
+  </si>
+  <si>
+    <t>Vu Thi Dung</t>
+  </si>
+  <si>
+    <t>TISGVQ</t>
+  </si>
+  <si>
+    <t>Do Anh Dung</t>
+  </si>
+  <si>
+    <t>EVYIE7</t>
+  </si>
+  <si>
+    <t>Do Thi Nam</t>
+  </si>
+  <si>
+    <t>R128XK</t>
+  </si>
+  <si>
+    <t>Tran Khanh Lan</t>
+  </si>
+  <si>
+    <t>E72W5H</t>
+  </si>
+  <si>
+    <t>Vu Duc Lan</t>
+  </si>
+  <si>
+    <t>TIR52G</t>
+  </si>
+  <si>
+    <t>Do Thuy Trang</t>
+  </si>
+  <si>
+    <t>UA9ILP</t>
+  </si>
+  <si>
+    <t>Le Minh Hieu</t>
+  </si>
+  <si>
+    <t>3EHBM2</t>
+  </si>
+  <si>
+    <t>Do Duc Khanh</t>
+  </si>
+  <si>
+    <t>ROPHNH</t>
+  </si>
+  <si>
+    <t>Pham Thi Tuan</t>
+  </si>
+  <si>
+    <t>GULKJX</t>
+  </si>
+  <si>
+    <t>Le Khanh Lan</t>
+  </si>
+  <si>
+    <t>52SB1P</t>
+  </si>
+  <si>
+    <t>Bui Anh Lan</t>
+  </si>
+  <si>
+    <t>W7PHJS</t>
+  </si>
+  <si>
+    <t>Tran Minh Lan</t>
+  </si>
+  <si>
+    <t>6VPKEC</t>
+  </si>
+  <si>
+    <t>Do Duc Nam</t>
+  </si>
+  <si>
+    <t>CMNHQL</t>
+  </si>
+  <si>
+    <t>Pham Thanh Hoa</t>
+  </si>
+  <si>
+    <t>KMI1HV</t>
+  </si>
+  <si>
+    <t>Tran Quang Hoa</t>
+  </si>
+  <si>
+    <t>DQC03O</t>
+  </si>
+  <si>
+    <t>Do Van Linh</t>
+  </si>
+  <si>
+    <t>VP2LLM</t>
+  </si>
+  <si>
+    <t>Pham Thi Hoa</t>
+  </si>
+  <si>
+    <t>IVH5ZT</t>
+  </si>
+  <si>
+    <t>Vu Van Nam</t>
+  </si>
+  <si>
+    <t>UE6D5Y</t>
+  </si>
+  <si>
+    <t>Le Phuong Khanh</t>
+  </si>
+  <si>
+    <t>LOFPKB</t>
+  </si>
+  <si>
+    <t>Vu Thuy Lan</t>
+  </si>
+  <si>
+    <t>1U1QRH</t>
+  </si>
+  <si>
+    <t>Do Minh Tuan</t>
+  </si>
+  <si>
+    <t>XCJ41Z</t>
+  </si>
+  <si>
+    <t>Le Khanh Khanh</t>
+  </si>
+  <si>
+    <t>PIP5Y7</t>
+  </si>
+  <si>
+    <t>Nguyen Thuy Linh</t>
+  </si>
+  <si>
+    <t>Z1RBH0</t>
+  </si>
+  <si>
+    <t>Do Anh Khanh</t>
+  </si>
+  <si>
+    <t>H3QUJ3</t>
+  </si>
+  <si>
+    <t>Le Khanh Nam</t>
+  </si>
+  <si>
+    <t>JMKWOD</t>
+  </si>
+  <si>
+    <t>Pham Phuong Tuan</t>
+  </si>
+  <si>
+    <t>3EAW85</t>
+  </si>
+  <si>
+    <t>Tran Duc Trang</t>
+  </si>
+  <si>
+    <t>RUTV82</t>
+  </si>
+  <si>
+    <t>Vo Anh Nam</t>
+  </si>
+  <si>
+    <t>S7N3S4</t>
+  </si>
+  <si>
+    <t>Vo Thuy Duy</t>
+  </si>
+  <si>
+    <t>5886HU</t>
+  </si>
+  <si>
+    <t>Vo Anh Lan</t>
+  </si>
+  <si>
+    <t>KQ090B</t>
+  </si>
+  <si>
+    <t>Dang Khanh Dung</t>
+  </si>
+  <si>
+    <t>SNHNUD</t>
+  </si>
+  <si>
+    <t>Bui Quang Tuan</t>
+  </si>
+  <si>
+    <t>ROYKGQ</t>
+  </si>
+  <si>
+    <t>Hoang Thi Lan</t>
+  </si>
+  <si>
+    <t>VU886L</t>
+  </si>
+  <si>
+    <t>BDHS88</t>
+  </si>
+  <si>
+    <t>Nguyen Van Hoa</t>
+  </si>
+  <si>
+    <t>V4O3LP</t>
+  </si>
+  <si>
+    <t>Le Quang Hieu</t>
+  </si>
+  <si>
+    <t>VD5NTY</t>
+  </si>
+  <si>
+    <t>Pham Quang Lan</t>
+  </si>
+  <si>
+    <t>YHPQSF</t>
+  </si>
+  <si>
+    <t>Do Duc Trang</t>
+  </si>
+  <si>
+    <t>WPM7IT</t>
+  </si>
+  <si>
+    <t>Vo Van Khanh</t>
+  </si>
+  <si>
+    <t>0P6IYI</t>
+  </si>
+  <si>
+    <t>Bui Minh Hieu</t>
+  </si>
+  <si>
+    <t>7T5JPL</t>
+  </si>
+  <si>
+    <t>Nguyen Van Hieu</t>
+  </si>
+  <si>
+    <t>OPMTCC</t>
+  </si>
+  <si>
+    <t>Vo Van Lan</t>
+  </si>
+  <si>
+    <t>2SRD91</t>
+  </si>
+  <si>
+    <t>Dang Duc Trang</t>
+  </si>
+  <si>
+    <t>06UU5H</t>
+  </si>
+  <si>
+    <t>Hoang Minh Hoa</t>
+  </si>
+  <si>
+    <t>NZT9MM</t>
+  </si>
+  <si>
+    <t>Pham Quang Hoa</t>
+  </si>
+  <si>
+    <t>7OJ847</t>
+  </si>
+  <si>
+    <t>Do Khanh Dung</t>
+  </si>
+  <si>
+    <t>J16ZMO</t>
+  </si>
+  <si>
+    <t>Pham Van Hoa</t>
+  </si>
+  <si>
+    <t>TX8LEE</t>
+  </si>
+  <si>
+    <t>Vu Quang Tuan</t>
+  </si>
+  <si>
+    <t>M1SCVN</t>
+  </si>
+  <si>
+    <t>Do Khanh Hoa</t>
+  </si>
+  <si>
+    <t>H9S24K</t>
+  </si>
+  <si>
+    <t>Vo Duc Hieu</t>
+  </si>
+  <si>
+    <t>T7K4YC</t>
+  </si>
+  <si>
+    <t>Dang Thuy Tuan</t>
+  </si>
+  <si>
+    <t>8VTQ9L</t>
+  </si>
+  <si>
+    <t>Dang Quang Nam</t>
+  </si>
+  <si>
+    <t>NC7GID</t>
+  </si>
+  <si>
+    <t>Nguyen Khanh Duy</t>
+  </si>
+  <si>
+    <t>N3PC1H</t>
+  </si>
+  <si>
+    <t>Pham Anh Duy</t>
+  </si>
+  <si>
+    <t>0Z61WU</t>
+  </si>
+  <si>
+    <t>Le Thi Khanh</t>
+  </si>
+  <si>
+    <t>L5OG1G</t>
+  </si>
+  <si>
+    <t>Le Anh Tuan</t>
+  </si>
+  <si>
+    <t>J51N7V</t>
+  </si>
+  <si>
+    <t>Nguyen Thuy Khanh</t>
+  </si>
+  <si>
+    <t>48C7CE</t>
+  </si>
+  <si>
+    <t>Pham Van Linh</t>
+  </si>
+  <si>
+    <t>IDVS1M</t>
+  </si>
+  <si>
+    <t>Le Duc Trang</t>
+  </si>
+  <si>
+    <t>P6UVT9</t>
+  </si>
+  <si>
+    <t>Vu Khanh Tuan</t>
+  </si>
+  <si>
+    <t>B5XHSL</t>
+  </si>
+  <si>
+    <t>Dang Phuong Nam</t>
+  </si>
+  <si>
+    <t>IBP77O</t>
+  </si>
+  <si>
+    <t>Vu Van Linh</t>
+  </si>
+  <si>
+    <t>SLP9CJ</t>
+  </si>
+  <si>
+    <t>Nguyen Thanh Tuan</t>
+  </si>
+  <si>
+    <t>SHRVZJ</t>
+  </si>
+  <si>
+    <t>Hoang Khanh Lan</t>
+  </si>
+  <si>
+    <t>NDL4N2</t>
+  </si>
+  <si>
+    <t>Tran Thi Hieu</t>
+  </si>
+  <si>
+    <t>CICAQN</t>
+  </si>
+  <si>
+    <t>Dang Minh Hieu</t>
+  </si>
+  <si>
+    <t>D2M5IJ</t>
+  </si>
+  <si>
+    <t>Dang Thuy Hoa</t>
+  </si>
+  <si>
+    <t>10E2YY</t>
+  </si>
+  <si>
+    <t>Do Khanh Trang</t>
+  </si>
+  <si>
+    <t>DP9O7I</t>
+  </si>
+  <si>
+    <t>Vu Khanh Duy</t>
+  </si>
+  <si>
+    <t>W25B5V</t>
+  </si>
+  <si>
+    <t>Hoang Thi Nam</t>
+  </si>
+  <si>
+    <t>YTCYJ3</t>
+  </si>
+  <si>
+    <t>Tran Thuy Lan</t>
+  </si>
+  <si>
+    <t>FLG21W</t>
+  </si>
+  <si>
+    <t>Hoang Thanh Tuan</t>
+  </si>
+  <si>
+    <t>560MWI</t>
+  </si>
+  <si>
+    <t>Dang Thuy Duy</t>
+  </si>
+  <si>
+    <t>CQB5KQ</t>
+  </si>
+  <si>
+    <t>Dang Thi Tuan</t>
+  </si>
+  <si>
+    <t>PKIUEP</t>
+  </si>
+  <si>
+    <t>Bui Van Hieu</t>
+  </si>
+  <si>
+    <t>NLO47N</t>
+  </si>
+  <si>
+    <t>Le Minh Tuan</t>
+  </si>
+  <si>
+    <t>NDSHUA</t>
+  </si>
+  <si>
+    <t>Dang Thanh Lan</t>
+  </si>
+  <si>
+    <t>UZ8XE5</t>
+  </si>
+  <si>
+    <t>Vo Khanh Khanh</t>
+  </si>
+  <si>
+    <t>DZULSL</t>
+  </si>
+  <si>
+    <t>Do Anh Lan</t>
+  </si>
+  <si>
+    <t>GCQ1K0</t>
+  </si>
+  <si>
+    <t>Dang Khanh Khanh</t>
+  </si>
+  <si>
+    <t>BDTSCX</t>
+  </si>
+  <si>
+    <t>Vo Van Nam</t>
+  </si>
+  <si>
+    <t>5DZ8MK</t>
+  </si>
+  <si>
+    <t>WAV5HU</t>
+  </si>
+  <si>
+    <t>Vo Minh Lan</t>
+  </si>
+  <si>
+    <t>XPY3IA</t>
+  </si>
+  <si>
+    <t>Pham Khanh Tuan</t>
+  </si>
+  <si>
+    <t>OWGPB8</t>
+  </si>
+  <si>
+    <t>Bui Phuong Nam</t>
+  </si>
+  <si>
+    <t>NWC9XU</t>
+  </si>
+  <si>
+    <t>Pham Duc Lan</t>
+  </si>
+  <si>
+    <t>VVFXJG</t>
+  </si>
+  <si>
+    <t>Vu Thi Duy</t>
+  </si>
+  <si>
+    <t>VR83D3</t>
+  </si>
+  <si>
+    <t>Hoang Anh Tuan</t>
+  </si>
+  <si>
+    <t>L10WJ1</t>
+  </si>
+  <si>
+    <t>Vu Duc Hoa</t>
+  </si>
+  <si>
+    <t>8XYCPN</t>
+  </si>
+  <si>
+    <t>NDNFHW</t>
+  </si>
+  <si>
+    <t>Do Minh Dung</t>
+  </si>
+  <si>
+    <t>CQCUN5</t>
+  </si>
+  <si>
+    <t>Z6U5BF</t>
+  </si>
+  <si>
+    <t>Le Thanh Hieu</t>
+  </si>
+  <si>
+    <t>4STJJ1</t>
+  </si>
+  <si>
+    <t>Nguyen Anh Duy</t>
+  </si>
+  <si>
+    <t>BY42WA</t>
+  </si>
+  <si>
+    <t>Hoang Duc Hoa</t>
+  </si>
+  <si>
+    <t>IWI86X</t>
+  </si>
+  <si>
+    <t>Nguyen Minh Khanh</t>
+  </si>
+  <si>
+    <t>S0JKT0</t>
+  </si>
+  <si>
+    <t>Pham Thanh Linh</t>
+  </si>
+  <si>
+    <t>90AAEI</t>
+  </si>
+  <si>
+    <t>Vu Khanh Hoa</t>
+  </si>
+  <si>
+    <t>WC9395</t>
+  </si>
+  <si>
+    <t>Do Thanh Lan</t>
+  </si>
+  <si>
+    <t>TS1ACP</t>
+  </si>
+  <si>
+    <t>Hoang Khanh Linh</t>
+  </si>
+  <si>
+    <t>RRQOFV</t>
+  </si>
+  <si>
+    <t>Vo Minh Linh</t>
+  </si>
+  <si>
+    <t>TGDJ81</t>
+  </si>
+  <si>
+    <t>Vo Phuong Dung</t>
+  </si>
+  <si>
+    <t>4KKFWP</t>
+  </si>
+  <si>
+    <t>Vu Van Hoa</t>
+  </si>
+  <si>
+    <t>PR2JDJ</t>
+  </si>
+  <si>
+    <t>Vu Khanh Hieu</t>
+  </si>
+  <si>
+    <t>K0NNK0</t>
+  </si>
+  <si>
+    <t>Pham Anh Khanh</t>
+  </si>
+  <si>
+    <t>PBWMWB</t>
+  </si>
+  <si>
+    <t>Pham Quang Khanh</t>
+  </si>
+  <si>
+    <t>XJ3PSN</t>
+  </si>
+  <si>
+    <t>Bui Thi Lan</t>
+  </si>
+  <si>
+    <t>G68AGP</t>
+  </si>
+  <si>
+    <t>Hoang Phuong Nam</t>
+  </si>
+  <si>
+    <t>N3O8OA</t>
+  </si>
+  <si>
+    <t>Bui Thi Trang</t>
+  </si>
+  <si>
+    <t>W9NGU2</t>
+  </si>
+  <si>
+    <t>Nguyen Minh Linh</t>
+  </si>
+  <si>
+    <t>5NR8MX</t>
+  </si>
+  <si>
+    <t>IWLLJT</t>
+  </si>
+  <si>
+    <t>DYF4UV</t>
+  </si>
+  <si>
+    <t>Vo Anh Hieu</t>
+  </si>
+  <si>
+    <t>DE5UI1</t>
+  </si>
+  <si>
+    <t>Hoang Phuong Dung</t>
+  </si>
+  <si>
+    <t>X6C8EQ</t>
+  </si>
+  <si>
+    <t>Pham Thuy Lan</t>
+  </si>
+  <si>
+    <t>DYRC69</t>
+  </si>
+  <si>
+    <t>Nguyen Phuong Hoa</t>
+  </si>
+  <si>
+    <t>14W1TS</t>
+  </si>
+  <si>
+    <t>Do Phuong Hoa</t>
+  </si>
+  <si>
+    <t>I12IQG</t>
+  </si>
+  <si>
+    <t>Do Thi Linh</t>
+  </si>
+  <si>
+    <t>1SZ10E</t>
+  </si>
+  <si>
+    <t>Vu Thuy Duy</t>
+  </si>
+  <si>
+    <t>VPFZZK</t>
+  </si>
+  <si>
+    <t>Le Anh Trang</t>
+  </si>
+  <si>
+    <t>IUHAEL</t>
+  </si>
+  <si>
+    <t>Pham Phuong Khanh</t>
+  </si>
+  <si>
+    <t>PGZWWZ</t>
+  </si>
+  <si>
+    <t>Tran Anh Tuan</t>
+  </si>
+  <si>
+    <t>3QXWK1</t>
+  </si>
+  <si>
+    <t>Vu Thanh Nam</t>
+  </si>
+  <si>
+    <t>1EVBBJ</t>
+  </si>
+  <si>
+    <t>Tran Thanh Lan</t>
+  </si>
+  <si>
+    <t>R1BDH0</t>
+  </si>
+  <si>
+    <t>Vu Quang Nam</t>
+  </si>
+  <si>
+    <t>3YMQ56</t>
+  </si>
+  <si>
+    <t>Do Thuy Dung</t>
+  </si>
+  <si>
+    <t>MMGS7L</t>
+  </si>
+  <si>
+    <t>4H2YS9</t>
+  </si>
+  <si>
+    <t>Dang Minh Lan</t>
+  </si>
+  <si>
+    <t>KXBYGK</t>
+  </si>
+  <si>
+    <t>Vu Khanh Trang</t>
+  </si>
+  <si>
+    <t>13LUMS</t>
+  </si>
+  <si>
+    <t>Vu Thuy Tuan</t>
+  </si>
+  <si>
+    <t>RUD8G7</t>
+  </si>
+  <si>
+    <t>Hoang Thi Dung</t>
+  </si>
+  <si>
+    <t>0B2K9O</t>
+  </si>
+  <si>
+    <t>Tran Thi Linh</t>
+  </si>
+  <si>
+    <t>SCPOXO</t>
+  </si>
+  <si>
+    <t>Vu Minh Hieu</t>
+  </si>
+  <si>
+    <t>IKTDWR</t>
+  </si>
+  <si>
+    <t>PJ4O78</t>
+  </si>
+  <si>
+    <t>Nguyen Thuy Trang</t>
+  </si>
+  <si>
+    <t>VDIN0G</t>
+  </si>
+  <si>
+    <t>Tran Quang Linh</t>
+  </si>
+  <si>
+    <t>VNI5KG</t>
+  </si>
+  <si>
+    <t>Bui Thi Tuan</t>
+  </si>
+  <si>
+    <t>GD0P5H</t>
+  </si>
+  <si>
+    <t>Do Quang Nam</t>
+  </si>
+  <si>
+    <t>N1K6W6</t>
+  </si>
+  <si>
+    <t>Dang Duc Lan</t>
+  </si>
+  <si>
+    <t>Q3RDNS</t>
+  </si>
+  <si>
+    <t>Nguyen Thi Nam</t>
+  </si>
+  <si>
+    <t>44EAM9</t>
+  </si>
+  <si>
+    <t>Vo Van Trang</t>
+  </si>
+  <si>
+    <t>DNLOUZ</t>
+  </si>
+  <si>
+    <t>Dang Quang Dung</t>
+  </si>
+  <si>
+    <t>0PZCM9</t>
+  </si>
+  <si>
+    <t>Pham Van Lan</t>
+  </si>
+  <si>
+    <t>HWYH0X</t>
+  </si>
+  <si>
+    <t>Hoang Thuy Lan</t>
+  </si>
+  <si>
+    <t>FDCFUW</t>
+  </si>
+  <si>
+    <t>Vo Khanh Nam</t>
+  </si>
+  <si>
+    <t>6GD7RZ</t>
+  </si>
+  <si>
+    <t>Vu Duc Nam</t>
+  </si>
+  <si>
+    <t>IMEH0R</t>
+  </si>
+  <si>
+    <t>4ED5KZ</t>
+  </si>
+  <si>
+    <t>Le Thanh Hoa</t>
+  </si>
+  <si>
+    <t>VMKA8D</t>
+  </si>
+  <si>
+    <t>Pham Minh Khanh</t>
+  </si>
+  <si>
+    <t>H48CXM</t>
+  </si>
+  <si>
+    <t>Hoang Khanh Hieu</t>
+  </si>
+  <si>
+    <t>F6C6SZ</t>
+  </si>
+  <si>
+    <t>Nguyen Anh Dung</t>
+  </si>
+  <si>
+    <t>SLBLFX</t>
+  </si>
+  <si>
+    <t>Hoang Phuong Duy</t>
+  </si>
+  <si>
+    <t>2GMU5I</t>
+  </si>
+  <si>
+    <t>V8PUDQ</t>
+  </si>
+  <si>
+    <t>Vo Phuong Linh</t>
+  </si>
+  <si>
+    <t>IISDBE</t>
+  </si>
+  <si>
+    <t>Do Thanh Hieu</t>
+  </si>
+  <si>
+    <t>T1XWW7</t>
+  </si>
+  <si>
+    <t>Hoang Van Hieu</t>
+  </si>
+  <si>
+    <t>NCRVGO</t>
+  </si>
+  <si>
+    <t>0B0O79</t>
+  </si>
+  <si>
+    <t>Vu Minh Duy</t>
+  </si>
+  <si>
+    <t>TN330V</t>
+  </si>
+  <si>
+    <t>Tran Thuy Dung</t>
+  </si>
+  <si>
+    <t>N230OL</t>
+  </si>
+  <si>
+    <t>Do Minh Hoa</t>
+  </si>
+  <si>
+    <t>VN1T0N</t>
+  </si>
+  <si>
+    <t>Do Duc Dung</t>
+  </si>
+  <si>
+    <t>J165WY</t>
+  </si>
+  <si>
+    <t>Nguyen Thi Tuan</t>
+  </si>
+  <si>
+    <t>50XUQN</t>
+  </si>
+  <si>
+    <t>Vu Anh Tuan</t>
+  </si>
+  <si>
+    <t>GI3P9Y</t>
+  </si>
+  <si>
+    <t>Pham Duc Duy</t>
+  </si>
+  <si>
+    <t>2N544J</t>
+  </si>
+  <si>
+    <t>F2ZNV4</t>
+  </si>
+  <si>
+    <t>Nguyen Anh Tuan</t>
+  </si>
+  <si>
+    <t>8KXWGG</t>
+  </si>
+  <si>
+    <t>Bui Thanh Hieu</t>
+  </si>
+  <si>
+    <t>RSJK5E</t>
+  </si>
+  <si>
+    <t>T01Z8T</t>
+  </si>
+  <si>
+    <t>Vo Thuy Hoa</t>
+  </si>
+  <si>
+    <t>QV48Z6</t>
+  </si>
+  <si>
+    <t>Le Van Tuan</t>
+  </si>
+  <si>
+    <t>MHJ7NK</t>
+  </si>
+  <si>
+    <t>Hoang Quang Tuan</t>
+  </si>
+  <si>
+    <t>SS8CDT</t>
+  </si>
+  <si>
+    <t>Nguyen Phuong Dung</t>
+  </si>
+  <si>
+    <t>PSQGEI</t>
+  </si>
+  <si>
+    <t>Bui Quang Hieu</t>
+  </si>
+  <si>
+    <t>SCHK3P</t>
+  </si>
+  <si>
+    <t>Le Khanh Tuan</t>
+  </si>
+  <si>
+    <t>7YVOUH</t>
+  </si>
+  <si>
+    <t>Vu Khanh Linh</t>
+  </si>
+  <si>
+    <t>SZEOOZ</t>
+  </si>
+  <si>
+    <t>Bui Van Nam</t>
+  </si>
+  <si>
+    <t>KDSFW2</t>
+  </si>
+  <si>
+    <t>Do Thanh Nam</t>
+  </si>
+  <si>
+    <t>RGQUY7</t>
+  </si>
+  <si>
+    <t>Tran Thi Tuan</t>
+  </si>
+  <si>
+    <t>R1CBDO</t>
+  </si>
+  <si>
+    <t>Hoang Thuy Tuan</t>
+  </si>
+  <si>
+    <t>4FAQ3Z</t>
+  </si>
+  <si>
+    <t>Do Duc Hieu</t>
+  </si>
+  <si>
+    <t>8PFJPG</t>
+  </si>
+  <si>
+    <t>Tran Thanh Trang</t>
+  </si>
+  <si>
+    <t>3ZN0XC</t>
+  </si>
+  <si>
+    <t>Pham Thuy Tuan</t>
+  </si>
+  <si>
+    <t>5I0X1A</t>
+  </si>
+  <si>
+    <t>YBL6W3</t>
+  </si>
+  <si>
+    <t>Tran Thanh Nam</t>
+  </si>
+  <si>
+    <t>52L16X</t>
+  </si>
+  <si>
+    <t>N6DJM6</t>
+  </si>
+  <si>
+    <t>Bui Thanh Dung</t>
+  </si>
+  <si>
+    <t>CJ78UJ</t>
+  </si>
+  <si>
+    <t>Tran Minh Hoa</t>
+  </si>
+  <si>
+    <t>3ACM4R</t>
+  </si>
+  <si>
+    <t>I1PZI8</t>
+  </si>
+  <si>
+    <t>Vu Quang Khanh</t>
+  </si>
+  <si>
+    <t>P8WVUI</t>
+  </si>
+  <si>
+    <t>Dang Thanh Trang</t>
+  </si>
+  <si>
+    <t>H10EPG</t>
+  </si>
+  <si>
+    <t>Le Thanh Nam</t>
+  </si>
+  <si>
+    <t>R1HFKF</t>
+  </si>
+  <si>
+    <t>Pham Phuong Duy</t>
+  </si>
+  <si>
+    <t>3PRBU4</t>
+  </si>
+  <si>
+    <t>Tran Quang Hieu</t>
+  </si>
+  <si>
+    <t>0VJAXW</t>
+  </si>
+  <si>
+    <t>MGCSQ8</t>
+  </si>
+  <si>
+    <t>Tran Minh Nam</t>
+  </si>
+  <si>
+    <t>OOPIJ4</t>
+  </si>
+  <si>
+    <t>Nguyen Thi Trang</t>
+  </si>
+  <si>
+    <t>1GFC6V</t>
+  </si>
+  <si>
+    <t>Pham Thi Linh</t>
   </si>
 </sst>
 </file>
@@ -17364,7 +18526,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -17387,11 +18549,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -17434,6 +18611,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -63498,7 +64678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6111EA-E636-DC49-8BB0-3D4FAB2D2279}">
   <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -66716,4 +67896,2836 @@
   <autoFilter ref="A1:F160" xr:uid="{FD6111EA-E636-DC49-8BB0-3D4FAB2D2279}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07300C0E-610D-0345-9751-4C681227A031}">
+  <dimension ref="A1:D201"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="15" t="s">
+        <v>5753</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>5754</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>5755</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>5756</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>5757</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5758</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1989</v>
+      </c>
+      <c r="D2" s="3">
+        <v>8.91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>5759</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5760</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1971</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>5761</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5762</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1973</v>
+      </c>
+      <c r="D4" s="3">
+        <v>9.91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>5763</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5764</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1971</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3" t="s">
+        <v>5765</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5766</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1990</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
+        <v>5767</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5768</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1982</v>
+      </c>
+      <c r="D7" s="3">
+        <v>7.93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3" t="s">
+        <v>5769</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5770</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1998</v>
+      </c>
+      <c r="D8" s="3">
+        <v>9.4700000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3" t="s">
+        <v>5771</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5772</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1983</v>
+      </c>
+      <c r="D9" s="3">
+        <v>9.36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
+        <v>5773</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5774</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1992</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>5775</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>5776</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1982</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4.0199999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3" t="s">
+        <v>5777</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>5778</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1981</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3" t="s">
+        <v>5779</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>5780</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1960</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
+        <v>5781</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>5782</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1963</v>
+      </c>
+      <c r="D14" s="3">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3" t="s">
+        <v>5783</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>5784</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1980</v>
+      </c>
+      <c r="D15" s="3">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3" t="s">
+        <v>5785</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>5786</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1966</v>
+      </c>
+      <c r="D16" s="3">
+        <v>7.98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3" t="s">
+        <v>5787</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>5788</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1977</v>
+      </c>
+      <c r="D17" s="3">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="3" t="s">
+        <v>5789</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>5790</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1979</v>
+      </c>
+      <c r="D18" s="3">
+        <v>8.26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3" t="s">
+        <v>5791</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>5792</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1961</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="3" t="s">
+        <v>5793</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>5794</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1983</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="3" t="s">
+        <v>5795</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>5796</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1972</v>
+      </c>
+      <c r="D21" s="3">
+        <v>9.18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="3" t="s">
+        <v>5797</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>5798</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1981</v>
+      </c>
+      <c r="D22" s="3">
+        <v>6.03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3" t="s">
+        <v>5799</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>5800</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1980</v>
+      </c>
+      <c r="D23" s="3">
+        <v>6.71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3" t="s">
+        <v>5801</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>5802</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1964</v>
+      </c>
+      <c r="D24" s="3">
+        <v>7.01</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="3" t="s">
+        <v>5803</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>5804</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1982</v>
+      </c>
+      <c r="D25" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3" t="s">
+        <v>5805</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>5806</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1992</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="3" t="s">
+        <v>5807</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>5808</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1983</v>
+      </c>
+      <c r="D27" s="3">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="3" t="s">
+        <v>5809</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>5810</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D28" s="3">
+        <v>5.51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="3" t="s">
+        <v>5811</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>5812</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1965</v>
+      </c>
+      <c r="D29" s="3">
+        <v>6.66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="3" t="s">
+        <v>5813</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>5814</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1993</v>
+      </c>
+      <c r="D30" s="3">
+        <v>5.21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="3" t="s">
+        <v>5815</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>5816</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1963</v>
+      </c>
+      <c r="D31" s="3">
+        <v>4.03</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="3" t="s">
+        <v>5817</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>5818</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1990</v>
+      </c>
+      <c r="D32" s="3">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="3" t="s">
+        <v>5819</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>5820</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1991</v>
+      </c>
+      <c r="D33" s="3">
+        <v>7.67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="3" t="s">
+        <v>5821</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>5822</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1971</v>
+      </c>
+      <c r="D34" s="3">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="3" t="s">
+        <v>5823</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>5824</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1996</v>
+      </c>
+      <c r="D35" s="3">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="3" t="s">
+        <v>5825</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>5826</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1981</v>
+      </c>
+      <c r="D36" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="3" t="s">
+        <v>5827</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>5828</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1997</v>
+      </c>
+      <c r="D37" s="3">
+        <v>6.72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="3" t="s">
+        <v>5829</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>5828</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1967</v>
+      </c>
+      <c r="D38" s="3">
+        <v>6.69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="3" t="s">
+        <v>5830</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>5831</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1992</v>
+      </c>
+      <c r="D39" s="3">
+        <v>6.44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="3" t="s">
+        <v>5832</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>5833</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1999</v>
+      </c>
+      <c r="D40" s="3">
+        <v>7.29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="3" t="s">
+        <v>5834</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>5835</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1981</v>
+      </c>
+      <c r="D41" s="3">
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="3" t="s">
+        <v>5836</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>5837</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1971</v>
+      </c>
+      <c r="D42" s="3">
+        <v>8.06</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="3" t="s">
+        <v>5838</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>5839</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1967</v>
+      </c>
+      <c r="D43" s="3">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="3" t="s">
+        <v>5840</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>5841</v>
+      </c>
+      <c r="C44" s="3">
+        <v>1997</v>
+      </c>
+      <c r="D44" s="3">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="3" t="s">
+        <v>5842</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>5843</v>
+      </c>
+      <c r="C45" s="3">
+        <v>1987</v>
+      </c>
+      <c r="D45" s="3">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="3" t="s">
+        <v>5844</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>5845</v>
+      </c>
+      <c r="C46" s="3">
+        <v>1970</v>
+      </c>
+      <c r="D46" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="3" t="s">
+        <v>5846</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>5847</v>
+      </c>
+      <c r="C47" s="3">
+        <v>1996</v>
+      </c>
+      <c r="D47" s="3">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="3" t="s">
+        <v>5848</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>5849</v>
+      </c>
+      <c r="C48" s="3">
+        <v>1978</v>
+      </c>
+      <c r="D48" s="3">
+        <v>7.82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="3" t="s">
+        <v>5850</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>5851</v>
+      </c>
+      <c r="C49" s="3">
+        <v>1965</v>
+      </c>
+      <c r="D49" s="3">
+        <v>9.14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="3" t="s">
+        <v>5852</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>5853</v>
+      </c>
+      <c r="C50" s="3">
+        <v>1974</v>
+      </c>
+      <c r="D50" s="3">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="3" t="s">
+        <v>5854</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>5855</v>
+      </c>
+      <c r="C51" s="3">
+        <v>1975</v>
+      </c>
+      <c r="D51" s="3">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="3" t="s">
+        <v>5856</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>5857</v>
+      </c>
+      <c r="C52" s="3">
+        <v>1984</v>
+      </c>
+      <c r="D52" s="3">
+        <v>7.92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="3" t="s">
+        <v>5858</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>5859</v>
+      </c>
+      <c r="C53" s="3">
+        <v>1964</v>
+      </c>
+      <c r="D53" s="3">
+        <v>8.36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="3" t="s">
+        <v>5860</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>5861</v>
+      </c>
+      <c r="C54" s="3">
+        <v>1974</v>
+      </c>
+      <c r="D54" s="3">
+        <v>6.87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="3" t="s">
+        <v>5862</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>5863</v>
+      </c>
+      <c r="C55" s="3">
+        <v>1973</v>
+      </c>
+      <c r="D55" s="3">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="3" t="s">
+        <v>5864</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>5865</v>
+      </c>
+      <c r="C56" s="3">
+        <v>1982</v>
+      </c>
+      <c r="D56" s="3">
+        <v>3.26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="3" t="s">
+        <v>5866</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>5867</v>
+      </c>
+      <c r="C57" s="3">
+        <v>1991</v>
+      </c>
+      <c r="D57" s="3">
+        <v>3.77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="3" t="s">
+        <v>5868</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>5869</v>
+      </c>
+      <c r="C58" s="3">
+        <v>1988</v>
+      </c>
+      <c r="D58" s="3">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="3" t="s">
+        <v>5870</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>5871</v>
+      </c>
+      <c r="C59" s="3">
+        <v>1973</v>
+      </c>
+      <c r="D59" s="3">
+        <v>5.51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="3" t="s">
+        <v>5872</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>5873</v>
+      </c>
+      <c r="C60" s="3">
+        <v>1997</v>
+      </c>
+      <c r="D60" s="3">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="3" t="s">
+        <v>5874</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>5875</v>
+      </c>
+      <c r="C61" s="3">
+        <v>1988</v>
+      </c>
+      <c r="D61" s="3">
+        <v>6.92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="3" t="s">
+        <v>5876</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>5877</v>
+      </c>
+      <c r="C62" s="3">
+        <v>1966</v>
+      </c>
+      <c r="D62" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="3" t="s">
+        <v>5878</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>5879</v>
+      </c>
+      <c r="C63" s="3">
+        <v>1961</v>
+      </c>
+      <c r="D63" s="3">
+        <v>5.08</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="3" t="s">
+        <v>5880</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>5881</v>
+      </c>
+      <c r="C64" s="3">
+        <v>1998</v>
+      </c>
+      <c r="D64" s="3">
+        <v>5.97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="3" t="s">
+        <v>5882</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>5883</v>
+      </c>
+      <c r="C65" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D65" s="3">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="3" t="s">
+        <v>5884</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>5885</v>
+      </c>
+      <c r="C66" s="3">
+        <v>1996</v>
+      </c>
+      <c r="D66" s="3">
+        <v>6.93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="3" t="s">
+        <v>5886</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>5887</v>
+      </c>
+      <c r="C67" s="3">
+        <v>1996</v>
+      </c>
+      <c r="D67" s="3">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="3" t="s">
+        <v>5888</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>5889</v>
+      </c>
+      <c r="C68" s="3">
+        <v>1962</v>
+      </c>
+      <c r="D68" s="3">
+        <v>9.9700000000000006</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="3" t="s">
+        <v>5890</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>5891</v>
+      </c>
+      <c r="C69" s="3">
+        <v>1972</v>
+      </c>
+      <c r="D69" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="3" t="s">
+        <v>5892</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>5893</v>
+      </c>
+      <c r="C70" s="3">
+        <v>1987</v>
+      </c>
+      <c r="D70" s="3">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="3" t="s">
+        <v>5894</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>5895</v>
+      </c>
+      <c r="C71" s="3">
+        <v>1977</v>
+      </c>
+      <c r="D71" s="3">
+        <v>9.34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="3" t="s">
+        <v>5896</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>5897</v>
+      </c>
+      <c r="C72" s="3">
+        <v>1995</v>
+      </c>
+      <c r="D72" s="3">
+        <v>4.3899999999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="3" t="s">
+        <v>5898</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>5899</v>
+      </c>
+      <c r="C73" s="3">
+        <v>1962</v>
+      </c>
+      <c r="D73" s="3">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="3" t="s">
+        <v>5900</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>5901</v>
+      </c>
+      <c r="C74" s="3">
+        <v>1966</v>
+      </c>
+      <c r="D74" s="3">
+        <v>6.81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="3" t="s">
+        <v>5902</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>5903</v>
+      </c>
+      <c r="C75" s="3">
+        <v>1973</v>
+      </c>
+      <c r="D75" s="3">
+        <v>5.96</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="3" t="s">
+        <v>5904</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>5905</v>
+      </c>
+      <c r="C76" s="3">
+        <v>1994</v>
+      </c>
+      <c r="D76" s="3">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="3" t="s">
+        <v>5906</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>5907</v>
+      </c>
+      <c r="C77" s="3">
+        <v>1998</v>
+      </c>
+      <c r="D77" s="3">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="3" t="s">
+        <v>5908</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>5909</v>
+      </c>
+      <c r="C78" s="3">
+        <v>1969</v>
+      </c>
+      <c r="D78" s="3">
+        <v>5.26</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="3" t="s">
+        <v>5910</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>5911</v>
+      </c>
+      <c r="C79" s="3">
+        <v>1990</v>
+      </c>
+      <c r="D79" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="3" t="s">
+        <v>5912</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>5913</v>
+      </c>
+      <c r="C80" s="3">
+        <v>1960</v>
+      </c>
+      <c r="D80" s="3">
+        <v>9.19</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="3" t="s">
+        <v>5914</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>5915</v>
+      </c>
+      <c r="C81" s="3">
+        <v>1987</v>
+      </c>
+      <c r="D81" s="3">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="3" t="s">
+        <v>5916</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>5917</v>
+      </c>
+      <c r="C82" s="3">
+        <v>1982</v>
+      </c>
+      <c r="D82" s="3">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="3" t="s">
+        <v>5918</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>5919</v>
+      </c>
+      <c r="C83" s="3">
+        <v>1968</v>
+      </c>
+      <c r="D83" s="3">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="3" t="s">
+        <v>5920</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>5921</v>
+      </c>
+      <c r="C84" s="3">
+        <v>1965</v>
+      </c>
+      <c r="D84" s="3">
+        <v>6.24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="3" t="s">
+        <v>5922</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>5923</v>
+      </c>
+      <c r="C85" s="3">
+        <v>1968</v>
+      </c>
+      <c r="D85" s="3">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="3" t="s">
+        <v>5924</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>5881</v>
+      </c>
+      <c r="C86" s="3">
+        <v>1985</v>
+      </c>
+      <c r="D86" s="3">
+        <v>7.92</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="3" t="s">
+        <v>5925</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>5926</v>
+      </c>
+      <c r="C87" s="3">
+        <v>1969</v>
+      </c>
+      <c r="D87" s="3">
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="3" t="s">
+        <v>5927</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>5928</v>
+      </c>
+      <c r="C88" s="3">
+        <v>1983</v>
+      </c>
+      <c r="D88" s="3">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="3" t="s">
+        <v>5929</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>5930</v>
+      </c>
+      <c r="C89" s="3">
+        <v>1990</v>
+      </c>
+      <c r="D89" s="3">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="3" t="s">
+        <v>5931</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>5932</v>
+      </c>
+      <c r="C90" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D90" s="3">
+        <v>5.21</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="3" t="s">
+        <v>5933</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>5934</v>
+      </c>
+      <c r="C91" s="3">
+        <v>1996</v>
+      </c>
+      <c r="D91" s="3">
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="3" t="s">
+        <v>5935</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>5936</v>
+      </c>
+      <c r="C92" s="3">
+        <v>1981</v>
+      </c>
+      <c r="D92" s="3">
+        <v>8.66</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="3" t="s">
+        <v>5937</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>5938</v>
+      </c>
+      <c r="C93" s="3">
+        <v>1966</v>
+      </c>
+      <c r="D93" s="3">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="3" t="s">
+        <v>5939</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>5770</v>
+      </c>
+      <c r="C94" s="3">
+        <v>1970</v>
+      </c>
+      <c r="D94" s="3">
+        <v>7.33</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="3" t="s">
+        <v>5940</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>5941</v>
+      </c>
+      <c r="C95" s="3">
+        <v>1969</v>
+      </c>
+      <c r="D95" s="3">
+        <v>7.55</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="3" t="s">
+        <v>5942</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>5820</v>
+      </c>
+      <c r="C96" s="3">
+        <v>1979</v>
+      </c>
+      <c r="D96" s="3">
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="3" t="s">
+        <v>5943</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>5944</v>
+      </c>
+      <c r="C97" s="3">
+        <v>1978</v>
+      </c>
+      <c r="D97" s="3">
+        <v>4.2300000000000004</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="3" t="s">
+        <v>5945</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>5946</v>
+      </c>
+      <c r="C98" s="3">
+        <v>1992</v>
+      </c>
+      <c r="D98" s="3">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="3" t="s">
+        <v>5947</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>5948</v>
+      </c>
+      <c r="C99" s="3">
+        <v>1964</v>
+      </c>
+      <c r="D99" s="3">
+        <v>6.21</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="3" t="s">
+        <v>5949</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>5950</v>
+      </c>
+      <c r="C100" s="3">
+        <v>1976</v>
+      </c>
+      <c r="D100" s="3">
+        <v>3.51</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="3" t="s">
+        <v>5951</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>5952</v>
+      </c>
+      <c r="C101" s="3">
+        <v>1987</v>
+      </c>
+      <c r="D101" s="3">
+        <v>8.44</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="3" t="s">
+        <v>5953</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>5954</v>
+      </c>
+      <c r="C102" s="3">
+        <v>1971</v>
+      </c>
+      <c r="D102" s="3">
+        <v>5.42</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="3" t="s">
+        <v>5955</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>5956</v>
+      </c>
+      <c r="C103" s="3">
+        <v>1975</v>
+      </c>
+      <c r="D103" s="3">
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="3" t="s">
+        <v>5957</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>5958</v>
+      </c>
+      <c r="C104" s="3">
+        <v>1972</v>
+      </c>
+      <c r="D104" s="3">
+        <v>6.28</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="3" t="s">
+        <v>5959</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>5960</v>
+      </c>
+      <c r="C105" s="3">
+        <v>1974</v>
+      </c>
+      <c r="D105" s="3">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="3" t="s">
+        <v>5961</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>5962</v>
+      </c>
+      <c r="C106" s="3">
+        <v>1997</v>
+      </c>
+      <c r="D106" s="3">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="3" t="s">
+        <v>5963</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>5964</v>
+      </c>
+      <c r="C107" s="3">
+        <v>1972</v>
+      </c>
+      <c r="D107" s="3">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="3" t="s">
+        <v>5965</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>5966</v>
+      </c>
+      <c r="C108" s="3">
+        <v>1961</v>
+      </c>
+      <c r="D108" s="3">
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="3" t="s">
+        <v>5967</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>5968</v>
+      </c>
+      <c r="C109" s="3">
+        <v>1973</v>
+      </c>
+      <c r="D109" s="3">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="3" t="s">
+        <v>5969</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>5970</v>
+      </c>
+      <c r="C110" s="3">
+        <v>1985</v>
+      </c>
+      <c r="D110" s="3">
+        <v>8.5299999999999994</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="3" t="s">
+        <v>5971</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>5972</v>
+      </c>
+      <c r="C111" s="3">
+        <v>1998</v>
+      </c>
+      <c r="D111" s="3">
+        <v>8.5299999999999994</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="3" t="s">
+        <v>5973</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>5974</v>
+      </c>
+      <c r="C112" s="3">
+        <v>1976</v>
+      </c>
+      <c r="D112" s="3">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="3" t="s">
+        <v>5975</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>5976</v>
+      </c>
+      <c r="C113" s="3">
+        <v>1985</v>
+      </c>
+      <c r="D113" s="3">
+        <v>6.11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="3" t="s">
+        <v>5977</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>5978</v>
+      </c>
+      <c r="C114" s="3">
+        <v>1961</v>
+      </c>
+      <c r="D114" s="3">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="3" t="s">
+        <v>5979</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>5788</v>
+      </c>
+      <c r="C115" s="3">
+        <v>1986</v>
+      </c>
+      <c r="D115" s="3">
+        <v>7.16</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="3" t="s">
+        <v>5980</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>5893</v>
+      </c>
+      <c r="C116" s="3">
+        <v>1985</v>
+      </c>
+      <c r="D116" s="3">
+        <v>7.77</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="3" t="s">
+        <v>5981</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>5982</v>
+      </c>
+      <c r="C117" s="3">
+        <v>1983</v>
+      </c>
+      <c r="D117" s="3">
+        <v>3.43</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="3" t="s">
+        <v>5983</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>5984</v>
+      </c>
+      <c r="C118" s="3">
+        <v>1991</v>
+      </c>
+      <c r="D118" s="3">
+        <v>7.29</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="3" t="s">
+        <v>5985</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>5986</v>
+      </c>
+      <c r="C119" s="3">
+        <v>1995</v>
+      </c>
+      <c r="D119" s="3">
+        <v>3.03</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="3" t="s">
+        <v>5987</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>5988</v>
+      </c>
+      <c r="C120" s="3">
+        <v>1962</v>
+      </c>
+      <c r="D120" s="3">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="3" t="s">
+        <v>5989</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>5990</v>
+      </c>
+      <c r="C121" s="3">
+        <v>1971</v>
+      </c>
+      <c r="D121" s="3">
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="3" t="s">
+        <v>5991</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>5992</v>
+      </c>
+      <c r="C122" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D122" s="3">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="3" t="s">
+        <v>5993</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>5994</v>
+      </c>
+      <c r="C123" s="3">
+        <v>1971</v>
+      </c>
+      <c r="D123" s="3">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="3" t="s">
+        <v>5995</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>5996</v>
+      </c>
+      <c r="C124" s="3">
+        <v>1983</v>
+      </c>
+      <c r="D124" s="3">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="3" t="s">
+        <v>5997</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>5998</v>
+      </c>
+      <c r="C125" s="3">
+        <v>1965</v>
+      </c>
+      <c r="D125" s="3">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="3" t="s">
+        <v>5999</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>6000</v>
+      </c>
+      <c r="C126" s="3">
+        <v>1983</v>
+      </c>
+      <c r="D126" s="3">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="3" t="s">
+        <v>6001</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>6002</v>
+      </c>
+      <c r="C127" s="3">
+        <v>1972</v>
+      </c>
+      <c r="D127" s="3">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="3" t="s">
+        <v>6003</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>6004</v>
+      </c>
+      <c r="C128" s="3">
+        <v>1966</v>
+      </c>
+      <c r="D128" s="3">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="3" t="s">
+        <v>6005</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>6006</v>
+      </c>
+      <c r="C129" s="3">
+        <v>1992</v>
+      </c>
+      <c r="D129" s="3">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="3" t="s">
+        <v>6007</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>6008</v>
+      </c>
+      <c r="C130" s="3">
+        <v>1994</v>
+      </c>
+      <c r="D130" s="3">
+        <v>9.65</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="3" t="s">
+        <v>6009</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>5938</v>
+      </c>
+      <c r="C131" s="3">
+        <v>1984</v>
+      </c>
+      <c r="D131" s="3">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="3" t="s">
+        <v>6010</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>6011</v>
+      </c>
+      <c r="C132" s="3">
+        <v>1990</v>
+      </c>
+      <c r="D132" s="3">
+        <v>7.78</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="3" t="s">
+        <v>6012</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>6013</v>
+      </c>
+      <c r="C133" s="3">
+        <v>1969</v>
+      </c>
+      <c r="D133" s="3">
+        <v>7.46</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="3" t="s">
+        <v>6014</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>6015</v>
+      </c>
+      <c r="C134" s="3">
+        <v>1985</v>
+      </c>
+      <c r="D134" s="3">
+        <v>9.07</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="3" t="s">
+        <v>6016</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>6017</v>
+      </c>
+      <c r="C135" s="3">
+        <v>1983</v>
+      </c>
+      <c r="D135" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="3" t="s">
+        <v>6018</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>6019</v>
+      </c>
+      <c r="C136" s="3">
+        <v>1961</v>
+      </c>
+      <c r="D136" s="3">
+        <v>4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="3" t="s">
+        <v>6020</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>6021</v>
+      </c>
+      <c r="C137" s="3">
+        <v>1965</v>
+      </c>
+      <c r="D137" s="3">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="3" t="s">
+        <v>6022</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>5938</v>
+      </c>
+      <c r="C138" s="3">
+        <v>1997</v>
+      </c>
+      <c r="D138" s="3">
+        <v>7.81</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="3" t="s">
+        <v>6023</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>6024</v>
+      </c>
+      <c r="C139" s="3">
+        <v>1986</v>
+      </c>
+      <c r="D139" s="3">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="3" t="s">
+        <v>6025</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>6026</v>
+      </c>
+      <c r="C140" s="3">
+        <v>1984</v>
+      </c>
+      <c r="D140" s="3">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="3" t="s">
+        <v>6027</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>6028</v>
+      </c>
+      <c r="C141" s="3">
+        <v>1988</v>
+      </c>
+      <c r="D141" s="3">
+        <v>8.49</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="3" t="s">
+        <v>6029</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>6030</v>
+      </c>
+      <c r="C142" s="3">
+        <v>1966</v>
+      </c>
+      <c r="D142" s="3">
+        <v>9.77</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="3" t="s">
+        <v>6031</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>6032</v>
+      </c>
+      <c r="C143" s="3">
+        <v>1989</v>
+      </c>
+      <c r="D143" s="3">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="3" t="s">
+        <v>6033</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>6034</v>
+      </c>
+      <c r="C144" s="3">
+        <v>1963</v>
+      </c>
+      <c r="D144" s="3">
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="3" t="s">
+        <v>6035</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>6036</v>
+      </c>
+      <c r="C145" s="3">
+        <v>1965</v>
+      </c>
+      <c r="D145" s="3">
+        <v>6.22</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="3" t="s">
+        <v>6037</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>6038</v>
+      </c>
+      <c r="C146" s="3">
+        <v>1983</v>
+      </c>
+      <c r="D146" s="3">
+        <v>7.84</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="3" t="s">
+        <v>6039</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>6040</v>
+      </c>
+      <c r="C147" s="3">
+        <v>1979</v>
+      </c>
+      <c r="D147" s="3">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="3" t="s">
+        <v>6041</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>6042</v>
+      </c>
+      <c r="C148" s="3">
+        <v>1983</v>
+      </c>
+      <c r="D148" s="3">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="3" t="s">
+        <v>6043</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>6044</v>
+      </c>
+      <c r="C149" s="3">
+        <v>1960</v>
+      </c>
+      <c r="D149" s="3">
+        <v>9.09</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="3" t="s">
+        <v>6045</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>6046</v>
+      </c>
+      <c r="C150" s="3">
+        <v>1982</v>
+      </c>
+      <c r="D150" s="3">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="3" t="s">
+        <v>6047</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>5861</v>
+      </c>
+      <c r="C151" s="3">
+        <v>1995</v>
+      </c>
+      <c r="D151" s="3">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="3" t="s">
+        <v>6048</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>6049</v>
+      </c>
+      <c r="C152" s="3">
+        <v>1992</v>
+      </c>
+      <c r="D152" s="3">
+        <v>8.11</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="3" t="s">
+        <v>6050</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>6051</v>
+      </c>
+      <c r="C153" s="3">
+        <v>1971</v>
+      </c>
+      <c r="D153" s="3">
+        <v>6.04</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="3" t="s">
+        <v>6052</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>6053</v>
+      </c>
+      <c r="C154" s="3">
+        <v>1988</v>
+      </c>
+      <c r="D154" s="3">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="3" t="s">
+        <v>6054</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>6055</v>
+      </c>
+      <c r="C155" s="3">
+        <v>1963</v>
+      </c>
+      <c r="D155" s="3">
+        <v>9.44</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="3" t="s">
+        <v>6056</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>6057</v>
+      </c>
+      <c r="C156" s="3">
+        <v>1977</v>
+      </c>
+      <c r="D156" s="3">
+        <v>8.4600000000000009</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="3" t="s">
+        <v>6058</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>5814</v>
+      </c>
+      <c r="C157" s="3">
+        <v>1980</v>
+      </c>
+      <c r="D157" s="3">
+        <v>7.21</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="3" t="s">
+        <v>6059</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>6060</v>
+      </c>
+      <c r="C158" s="3">
+        <v>1972</v>
+      </c>
+      <c r="D158" s="3">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="3" t="s">
+        <v>6061</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>6062</v>
+      </c>
+      <c r="C159" s="3">
+        <v>1987</v>
+      </c>
+      <c r="D159" s="3">
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="3" t="s">
+        <v>6063</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>6064</v>
+      </c>
+      <c r="C160" s="3">
+        <v>1986</v>
+      </c>
+      <c r="D160" s="3">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="3" t="s">
+        <v>6065</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>5764</v>
+      </c>
+      <c r="C161" s="3">
+        <v>1975</v>
+      </c>
+      <c r="D161" s="3">
+        <v>7.52</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="3" t="s">
+        <v>6066</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>6067</v>
+      </c>
+      <c r="C162" s="3">
+        <v>1996</v>
+      </c>
+      <c r="D162" s="3">
+        <v>8.2899999999999991</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="3" t="s">
+        <v>6068</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>6069</v>
+      </c>
+      <c r="C163" s="3">
+        <v>1996</v>
+      </c>
+      <c r="D163" s="3">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="3" t="s">
+        <v>6070</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>6071</v>
+      </c>
+      <c r="C164" s="3">
+        <v>1981</v>
+      </c>
+      <c r="D164" s="3">
+        <v>9.48</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="3" t="s">
+        <v>6072</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>6073</v>
+      </c>
+      <c r="C165" s="3">
+        <v>1968</v>
+      </c>
+      <c r="D165" s="3">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="3" t="s">
+        <v>6074</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>6075</v>
+      </c>
+      <c r="C166" s="3">
+        <v>1998</v>
+      </c>
+      <c r="D166" s="3">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="3" t="s">
+        <v>6076</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>6077</v>
+      </c>
+      <c r="C167" s="3">
+        <v>1974</v>
+      </c>
+      <c r="D167" s="3">
+        <v>5.48</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="3" t="s">
+        <v>6078</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>6079</v>
+      </c>
+      <c r="C168" s="3">
+        <v>1999</v>
+      </c>
+      <c r="D168" s="3">
+        <v>6.02</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="3" t="s">
+        <v>6080</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>5849</v>
+      </c>
+      <c r="C169" s="3">
+        <v>1967</v>
+      </c>
+      <c r="D169" s="3">
+        <v>8.23</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="3" t="s">
+        <v>6081</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>6082</v>
+      </c>
+      <c r="C170" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D170" s="3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" s="3" t="s">
+        <v>6083</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>6084</v>
+      </c>
+      <c r="C171" s="3">
+        <v>1962</v>
+      </c>
+      <c r="D171" s="3">
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" s="3" t="s">
+        <v>6085</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>5839</v>
+      </c>
+      <c r="C172" s="3">
+        <v>1989</v>
+      </c>
+      <c r="D172" s="3">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" s="3" t="s">
+        <v>6086</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>6087</v>
+      </c>
+      <c r="C173" s="3">
+        <v>1963</v>
+      </c>
+      <c r="D173" s="3">
+        <v>8.51</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="3" t="s">
+        <v>6088</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>6089</v>
+      </c>
+      <c r="C174" s="3">
+        <v>1997</v>
+      </c>
+      <c r="D174" s="3">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="3" t="s">
+        <v>6090</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>6091</v>
+      </c>
+      <c r="C175" s="3">
+        <v>1990</v>
+      </c>
+      <c r="D175" s="3">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="3" t="s">
+        <v>6092</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>6093</v>
+      </c>
+      <c r="C176" s="3">
+        <v>1964</v>
+      </c>
+      <c r="D176" s="3">
+        <v>3.62</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="3" t="s">
+        <v>6094</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>6095</v>
+      </c>
+      <c r="C177" s="3">
+        <v>1973</v>
+      </c>
+      <c r="D177" s="3">
+        <v>9.26</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" s="3" t="s">
+        <v>6096</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>6097</v>
+      </c>
+      <c r="C178" s="3">
+        <v>1980</v>
+      </c>
+      <c r="D178" s="3">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" s="3" t="s">
+        <v>6098</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>6099</v>
+      </c>
+      <c r="C179" s="3">
+        <v>1960</v>
+      </c>
+      <c r="D179" s="3">
+        <v>9.07</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" s="3" t="s">
+        <v>6100</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>6101</v>
+      </c>
+      <c r="C180" s="3">
+        <v>1988</v>
+      </c>
+      <c r="D180" s="3">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" s="3" t="s">
+        <v>6102</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>6103</v>
+      </c>
+      <c r="C181" s="3">
+        <v>1996</v>
+      </c>
+      <c r="D181" s="3">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" s="3" t="s">
+        <v>6104</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>6105</v>
+      </c>
+      <c r="C182" s="3">
+        <v>1961</v>
+      </c>
+      <c r="D182" s="3">
+        <v>9.2899999999999991</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" s="3" t="s">
+        <v>6106</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>6107</v>
+      </c>
+      <c r="C183" s="3">
+        <v>1975</v>
+      </c>
+      <c r="D183" s="3">
+        <v>6.86</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" s="3" t="s">
+        <v>6108</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>6109</v>
+      </c>
+      <c r="C184" s="3">
+        <v>1971</v>
+      </c>
+      <c r="D184" s="3">
+        <v>9.26</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" s="3" t="s">
+        <v>6110</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>6111</v>
+      </c>
+      <c r="C185" s="3">
+        <v>1990</v>
+      </c>
+      <c r="D185" s="3">
+        <v>6.62</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" s="3" t="s">
+        <v>6112</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>6113</v>
+      </c>
+      <c r="C186" s="3">
+        <v>1980</v>
+      </c>
+      <c r="D186" s="3">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" s="3" t="s">
+        <v>6114</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>6113</v>
+      </c>
+      <c r="C187" s="3">
+        <v>1989</v>
+      </c>
+      <c r="D187" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" s="3" t="s">
+        <v>6115</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>6116</v>
+      </c>
+      <c r="C188" s="3">
+        <v>1970</v>
+      </c>
+      <c r="D188" s="3">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" s="3" t="s">
+        <v>6117</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>6064</v>
+      </c>
+      <c r="C189" s="3">
+        <v>1982</v>
+      </c>
+      <c r="D189" s="3">
+        <v>8.39</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" s="3" t="s">
+        <v>6118</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>6119</v>
+      </c>
+      <c r="C190" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D190" s="3">
+        <v>8.61</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" s="3" t="s">
+        <v>6120</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>6121</v>
+      </c>
+      <c r="C191" s="3">
+        <v>1977</v>
+      </c>
+      <c r="D191" s="3">
+        <v>9.61</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" s="3" t="s">
+        <v>6122</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>6004</v>
+      </c>
+      <c r="C192" s="3">
+        <v>1972</v>
+      </c>
+      <c r="D192" s="3">
+        <v>4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" s="3" t="s">
+        <v>6123</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>6124</v>
+      </c>
+      <c r="C193" s="3">
+        <v>1989</v>
+      </c>
+      <c r="D193" s="3">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" s="3" t="s">
+        <v>6125</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>6126</v>
+      </c>
+      <c r="C194" s="3">
+        <v>1996</v>
+      </c>
+      <c r="D194" s="3">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" s="3" t="s">
+        <v>6127</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>6128</v>
+      </c>
+      <c r="C195" s="3">
+        <v>1982</v>
+      </c>
+      <c r="D195" s="3">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="3" t="s">
+        <v>6129</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>6130</v>
+      </c>
+      <c r="C196" s="3">
+        <v>1970</v>
+      </c>
+      <c r="D196" s="3">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" s="3" t="s">
+        <v>6131</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>6132</v>
+      </c>
+      <c r="C197" s="3">
+        <v>1969</v>
+      </c>
+      <c r="D197" s="3">
+        <v>4.2300000000000004</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="3" t="s">
+        <v>6133</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>6069</v>
+      </c>
+      <c r="C198" s="3">
+        <v>1966</v>
+      </c>
+      <c r="D198" s="3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="3" t="s">
+        <v>6134</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>6135</v>
+      </c>
+      <c r="C199" s="3">
+        <v>1977</v>
+      </c>
+      <c r="D199" s="3">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" s="3" t="s">
+        <v>6136</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>6137</v>
+      </c>
+      <c r="C200" s="3">
+        <v>1983</v>
+      </c>
+      <c r="D200" s="3">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" s="3" t="s">
+        <v>6138</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>6139</v>
+      </c>
+      <c r="C201" s="3">
+        <v>1964</v>
+      </c>
+      <c r="D201" s="3">
+        <v>5.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>